<commit_message>
[v2.0] Update with realistic, varied content (Excel)
</commit_message>
<xml_diff>
--- a/samples/google_display_ads_demo.xlsx
+++ b/samples/google_display_ads_demo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="174">
   <si>
     <t>Campaign</t>
   </si>
@@ -55,76 +55,82 @@
     <t>Call to Action</t>
   </si>
   <si>
-    <t>Display Campaign 1</t>
-  </si>
-  <si>
-    <t>Display Campaign 2</t>
-  </si>
-  <si>
-    <t>Display Campaign 3</t>
-  </si>
-  <si>
-    <t>Display Campaign 4</t>
-  </si>
-  <si>
-    <t>Ad Group 1</t>
-  </si>
-  <si>
-    <t>Ad Group 2</t>
-  </si>
-  <si>
-    <t>Ad Group 3</t>
-  </si>
-  <si>
-    <t>Ad Group 4</t>
-  </si>
-  <si>
-    <t>Ad Group 5</t>
-  </si>
-  <si>
-    <t>Ad Group 6</t>
-  </si>
-  <si>
-    <t>Ad Group 7</t>
-  </si>
-  <si>
-    <t>Ad Group 8</t>
-  </si>
-  <si>
-    <t>Ad Group 9</t>
-  </si>
-  <si>
-    <t>Ad Group 10</t>
-  </si>
-  <si>
-    <t>Ad Group 11</t>
-  </si>
-  <si>
-    <t>Ad Group 12</t>
-  </si>
-  <si>
-    <t>Ad Group 13</t>
-  </si>
-  <si>
-    <t>Ad Group 14</t>
-  </si>
-  <si>
-    <t>Ad Group 15</t>
-  </si>
-  <si>
-    <t>Ad Group 16</t>
-  </si>
-  <si>
-    <t>Ad Group 17</t>
-  </si>
-  <si>
-    <t>Ad Group 18</t>
-  </si>
-  <si>
-    <t>Ad Group 19</t>
-  </si>
-  <si>
-    <t>Ad Group 20</t>
+    <t>Display - Remarketing</t>
+  </si>
+  <si>
+    <t>Display - Prospecting</t>
+  </si>
+  <si>
+    <t>Display - Brand Awareness</t>
+  </si>
+  <si>
+    <t>Display - Conversion</t>
+  </si>
+  <si>
+    <t>Display - Brand</t>
+  </si>
+  <si>
+    <t>Display - Retargeting</t>
+  </si>
+  <si>
+    <t>CloudStore Pro - Ad Group 1</t>
+  </si>
+  <si>
+    <t>TaskFlow - Ad Group 2</t>
+  </si>
+  <si>
+    <t>EmailPro - Ad Group 3</t>
+  </si>
+  <si>
+    <t>SalesCentral - Ad Group 4</t>
+  </si>
+  <si>
+    <t>DataViz Analytics - Ad Group 5</t>
+  </si>
+  <si>
+    <t>MeetingHub - Ad Group 6</t>
+  </si>
+  <si>
+    <t>ContentAI - Ad Group 7</t>
+  </si>
+  <si>
+    <t>SocialBoost - Ad Group 8</t>
+  </si>
+  <si>
+    <t>SecureVault - Ad Group 9</t>
+  </si>
+  <si>
+    <t>QuickBooks Pro - Ad Group 10</t>
+  </si>
+  <si>
+    <t>CloudStore Pro - Ad Group 11</t>
+  </si>
+  <si>
+    <t>TaskFlow - Ad Group 12</t>
+  </si>
+  <si>
+    <t>EmailPro - Ad Group 13</t>
+  </si>
+  <si>
+    <t>SalesCentral - Ad Group 14</t>
+  </si>
+  <si>
+    <t>DataViz Analytics - Ad Group 15</t>
+  </si>
+  <si>
+    <t>MeetingHub - Ad Group 16</t>
+  </si>
+  <si>
+    <t>Business Intelligence - Premium</t>
+  </si>
+  <si>
+    <t>Email Hosting Premium</t>
+  </si>
+  <si>
+    <t>Project Management Tools</t>
+  </si>
+  <si>
+    <t>CRM Software New</t>
   </si>
   <si>
     <t>Display Ad 1</t>
@@ -190,16 +196,43 @@
     <t>Enabled</t>
   </si>
   <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>Save on Cloud Storage</t>
-  </si>
-  <si>
-    <t>AI-Powered Analytics</t>
-  </si>
-  <si>
-    <t>This is a very long short headline that exceeds limit</t>
+    <t>active</t>
+  </si>
+  <si>
+    <t>Secure Cloud Storage</t>
+  </si>
+  <si>
+    <t>Project Management Tool</t>
+  </si>
+  <si>
+    <t>Email Marketing Platform</t>
+  </si>
+  <si>
+    <t>All-in-One CRM</t>
+  </si>
+  <si>
+    <t>Business Intelligence</t>
+  </si>
+  <si>
+    <t>Video Conferencing</t>
+  </si>
+  <si>
+    <t>AI Writing Assistant</t>
+  </si>
+  <si>
+    <t>Social Media Manager</t>
+  </si>
+  <si>
+    <t>Password Manager</t>
+  </si>
+  <si>
+    <t>Accounting Software</t>
+  </si>
+  <si>
+    <t>Advanced Business Analytics</t>
+  </si>
+  <si>
+    <t>This is an extremely long short headline that definitely exceeds the thirty character limit</t>
   </si>
   <si>
     <t>Project Management</t>
@@ -208,64 +241,301 @@
     <t>CRM Software</t>
   </si>
   <si>
-    <t>Unlimited Cloud Storage for Teams - Start Free Trial Today</t>
-  </si>
-  <si>
-    <t>Transform Your Data Into Actionable Business Intelligence Fast</t>
-  </si>
-  <si>
-    <t>Get Professional Email Hosting with 24/7 Support</t>
-  </si>
-  <si>
-    <t>Streamline Your Workflow with Our Powerful Project Management Tools</t>
+    <t>Store and Share Files Securely - Start Free Trial</t>
+  </si>
+  <si>
+    <t>Manage Projects Efficiently with Real-Time Collaboration</t>
+  </si>
+  <si>
+    <t>Create Stunning Email Campaigns in Minutes - No Code Required</t>
+  </si>
+  <si>
+    <t>Transform Your Sales Process with AI-Powered CRM Software</t>
+  </si>
+  <si>
+    <t>Turn Data Into Insights with Beautiful Dashboards and Reports</t>
+  </si>
+  <si>
+    <t>Host HD Video Meetings with Up to 500 Participants</t>
+  </si>
+  <si>
+    <t>Generate High-Quality Content 10x Faster with AI</t>
+  </si>
+  <si>
+    <t>Schedule Posts Across All Platforms from One Dashboard</t>
+  </si>
+  <si>
+    <t>Keep All Your Passwords Safe with Military-Grade Encryption</t>
+  </si>
+  <si>
+    <t>Simplify Your Bookkeeping with Automated Accounting</t>
+  </si>
+  <si>
+    <t>Transform Your Business Data Into Actionable Insights with AI-Powered Analytics</t>
+  </si>
+  <si>
+    <t>Professional Email Hosting with 24/7 Support and Advanced Security Features</t>
+  </si>
+  <si>
+    <t>Streamline Your Workflow with Powerful Project Management Tools</t>
   </si>
   <si>
     <t>All-in-One CRM Solution for Growing Businesses</t>
   </si>
   <si>
-    <t>Secure, scalable storage for your business. 99.9% uptime guaranteed.</t>
-  </si>
-  <si>
-    <t>Real-time dashboards, predictive analytics, and automated reporting.</t>
-  </si>
-  <si>
-    <t>Reliable email hosting with advanced security features included.</t>
-  </si>
-  <si>
-    <t>Collaborate better, deliver faster. Try free for 30 days.</t>
-  </si>
-  <si>
-    <t>Manage customers, track sales, automate marketing. Start today!</t>
+    <t>99.9% uptime. Enterprise-grade security. Unlimited bandwidth.</t>
+  </si>
+  <si>
+    <t>Gantt charts, time tracking, team chat. Trusted by 50K+ teams.</t>
+  </si>
+  <si>
+    <t>Drag-and-drop builder. A/B testing. 99% deliverability rate.</t>
+  </si>
+  <si>
+    <t>Lead scoring, pipeline management, email integration. Free trial.</t>
+  </si>
+  <si>
+    <t>Real-time analytics. Custom visualizations. No SQL required.</t>
+  </si>
+  <si>
+    <t>Screen sharing, recording, breakout rooms. SOC 2 certified.</t>
+  </si>
+  <si>
+    <t>Blog posts, ads, emails. 50+ templates. Plagiarism-free.</t>
+  </si>
+  <si>
+    <t>Instagram, Facebook, Twitter, LinkedIn. Analytics included.</t>
+  </si>
+  <si>
+    <t>Auto-fill, secure sharing, dark web monitoring. Family plans.</t>
+  </si>
+  <si>
+    <t>Invoicing, expense tracking, tax prep. Used by 1M+ businesses.</t>
+  </si>
+  <si>
+    <t>Real-time dashboards, predictive analytics, automated reporting, data visualization.</t>
+  </si>
+  <si>
+    <t>Reliable email hosting with 99.9% uptime and enterprise-grade security.</t>
+  </si>
+  <si>
+    <t>Collaborate better, deliver faster. Gantt charts, time tracking, team chat.</t>
+  </si>
+  <si>
+    <t>Manage customers, track sales, automate marketing. Start free trial today!</t>
   </si>
   <si>
     <t>CloudStore Pro</t>
   </si>
   <si>
-    <t>Business Intelligence Solutions Inc</t>
+    <t>TaskFlow</t>
   </si>
   <si>
     <t>EmailPro</t>
   </si>
   <si>
-    <t>TaskFlow</t>
-  </si>
-  <si>
     <t>SalesCentral</t>
   </si>
   <si>
-    <t>https://example.com/landing</t>
-  </si>
-  <si>
-    <t>https://example.com/images/landscape.jpg</t>
-  </si>
-  <si>
-    <t>https://example.com/images/square.jpg</t>
-  </si>
-  <si>
-    <t>https://example.com/images/logo.png</t>
+    <t>DataViz Analytics</t>
+  </si>
+  <si>
+    <t>MeetingHub</t>
+  </si>
+  <si>
+    <t>ContentAI</t>
+  </si>
+  <si>
+    <t>SocialBoost</t>
+  </si>
+  <si>
+    <t>SecureVault</t>
+  </si>
+  <si>
+    <t>QuickBooks Pro</t>
+  </si>
+  <si>
+    <t>Business Intelligence Solutions International Inc</t>
+  </si>
+  <si>
+    <t>https://cloudstorepro.com/landing</t>
+  </si>
+  <si>
+    <t>https://taskflow.com/landing</t>
+  </si>
+  <si>
+    <t>https://emailpro.com/landing</t>
+  </si>
+  <si>
+    <t>https://salescentral.com/landing</t>
+  </si>
+  <si>
+    <t>https://datavizanalytics.com/landing</t>
+  </si>
+  <si>
+    <t>https://meetinghub.com/landing</t>
+  </si>
+  <si>
+    <t>https://contentai.com/landing</t>
+  </si>
+  <si>
+    <t>https://socialboost.com/landing</t>
+  </si>
+  <si>
+    <t>https://securevault.com/landing</t>
+  </si>
+  <si>
+    <t>https://quickbookspro.com/landing</t>
+  </si>
+  <si>
+    <t>https://businessintel.com/analytics</t>
+  </si>
+  <si>
+    <t>https://emailpro.com/business</t>
+  </si>
+  <si>
+    <t>https://salescentral.com/crm</t>
+  </si>
+  <si>
+    <t>https://cdn.cloudstorepro.com/images/landscape-1200x628.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.taskflow.com/images/landscape-1200x628.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.emailpro.com/images/landscape-1200x628.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.salescentral.com/images/landscape-1200x628.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.datavizanalytics.com/images/landscape-1200x628.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.meetinghub.com/images/landscape-1200x628.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.contentai.com/images/landscape-1200x628.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.socialboost.com/images/landscape-1200x628.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.securevault.com/images/landscape-1200x628.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.quickbookspro.com/images/landscape-1200x628.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.businessintel.com/images/landscape.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.emailpro.com/images/landscape.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.taskflow.com/images/landscape.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.salescentral.com/images/landscape.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.cloudstorepro.com/images/square-1200x1200.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.taskflow.com/images/square-1200x1200.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.emailpro.com/images/square-1200x1200.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.salescentral.com/images/square-1200x1200.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.datavizanalytics.com/images/square-1200x1200.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.meetinghub.com/images/square-1200x1200.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.contentai.com/images/square-1200x1200.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.socialboost.com/images/square-1200x1200.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.securevault.com/images/square-1200x1200.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.quickbookspro.com/images/square-1200x1200.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.businessintel.com/images/square.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.emailpro.com/images/square.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.taskflow.com/images/square.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.salescentral.com/images/square.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.cloudstorepro.com/images/logo-512x512.png</t>
+  </si>
+  <si>
+    <t>https://cdn.taskflow.com/images/logo-512x512.png</t>
+  </si>
+  <si>
+    <t>https://cdn.emailpro.com/images/logo-512x512.png</t>
+  </si>
+  <si>
+    <t>https://cdn.salescentral.com/images/logo-512x512.png</t>
+  </si>
+  <si>
+    <t>https://cdn.datavizanalytics.com/images/logo-512x512.png</t>
+  </si>
+  <si>
+    <t>https://cdn.meetinghub.com/images/logo-512x512.png</t>
+  </si>
+  <si>
+    <t>https://cdn.contentai.com/images/logo-512x512.png</t>
+  </si>
+  <si>
+    <t>https://cdn.socialboost.com/images/logo-512x512.png</t>
+  </si>
+  <si>
+    <t>https://cdn.securevault.com/images/logo-512x512.png</t>
+  </si>
+  <si>
+    <t>https://cdn.quickbookspro.com/images/logo-512x512.png</t>
+  </si>
+  <si>
+    <t>https://cdn.businessintel.com/images/logo.png</t>
+  </si>
+  <si>
+    <t>https://cdn.emailpro.com/images/logo.png</t>
+  </si>
+  <si>
+    <t>https://cdn.taskflow.com/images/logo.png</t>
+  </si>
+  <si>
+    <t>https://cdn.salescentral.com/images/logo.png</t>
+  </si>
+  <si>
+    <t>GET_QUOTE</t>
+  </si>
+  <si>
+    <t>SIGN_UP</t>
+  </si>
+  <si>
+    <t>DOWNLOAD</t>
   </si>
   <si>
     <t>LEARN_MORE</t>
+  </si>
+  <si>
+    <t>CONTACT_US</t>
   </si>
 </sst>
 </file>
@@ -688,163 +958,163 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="G2" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="H2" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>81</v>
+        <v>141</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>82</v>
+        <v>155</v>
       </c>
       <c r="M2" t="s">
-        <v>83</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="H3" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>80</v>
+        <v>128</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
       <c r="M3" t="s">
-        <v>83</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F4" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="H4" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>80</v>
+        <v>129</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>82</v>
+        <v>157</v>
       </c>
       <c r="M4" t="s">
-        <v>83</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="G5" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="H5" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>81</v>
+        <v>144</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>82</v>
+        <v>158</v>
       </c>
       <c r="M5" t="s">
-        <v>83</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -852,40 +1122,40 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="G6" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="H6" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>79</v>
+        <v>118</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>81</v>
+        <v>145</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>82</v>
+        <v>159</v>
       </c>
       <c r="M6" t="s">
-        <v>83</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -893,163 +1163,163 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="G7" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="H7" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>80</v>
+        <v>132</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>81</v>
+        <v>146</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>82</v>
+        <v>160</v>
       </c>
       <c r="M7" t="s">
-        <v>83</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E8" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="G8" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="H8" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>79</v>
+        <v>120</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>80</v>
+        <v>133</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>81</v>
+        <v>147</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>82</v>
+        <v>161</v>
       </c>
       <c r="M8" t="s">
-        <v>83</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="F9" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="G9" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="H9" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>80</v>
+        <v>134</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>81</v>
+        <v>148</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>82</v>
+        <v>162</v>
       </c>
       <c r="M9" t="s">
-        <v>83</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="F10" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="G10" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="H10" t="s">
-        <v>74</v>
+        <v>111</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>80</v>
+        <v>135</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>81</v>
+        <v>149</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>82</v>
+        <v>163</v>
       </c>
       <c r="M10" t="s">
-        <v>83</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1057,40 +1327,40 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="F11" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="G11" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="H11" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>79</v>
+        <v>123</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>80</v>
+        <v>136</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>81</v>
+        <v>150</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>82</v>
+        <v>164</v>
       </c>
       <c r="M11" t="s">
-        <v>83</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1098,163 +1368,163 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F12" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="G12" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="H12" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>81</v>
+        <v>141</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>82</v>
+        <v>155</v>
       </c>
       <c r="M12" t="s">
-        <v>83</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F13" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="G13" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="H13" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>80</v>
+        <v>128</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
       <c r="M13" t="s">
-        <v>83</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F14" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="H14" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>80</v>
+        <v>129</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>82</v>
+        <v>157</v>
       </c>
       <c r="M14" t="s">
-        <v>83</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E15" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F15" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="G15" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="H15" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>81</v>
+        <v>144</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>82</v>
+        <v>158</v>
       </c>
       <c r="M15" t="s">
-        <v>83</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1262,40 +1532,40 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F16" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="G16" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="H16" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>79</v>
+        <v>118</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>81</v>
+        <v>145</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>82</v>
+        <v>159</v>
       </c>
       <c r="M16" t="s">
-        <v>83</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -1303,40 +1573,40 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="F17" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="G17" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="H17" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>80</v>
+        <v>132</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>81</v>
+        <v>146</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>82</v>
+        <v>160</v>
       </c>
       <c r="M17" t="s">
-        <v>83</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -1344,160 +1614,160 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="F18" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="G18" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="H18" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>80</v>
+        <v>137</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>81</v>
+        <v>151</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>82</v>
+        <v>165</v>
       </c>
       <c r="M18" t="s">
-        <v>83</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="F19" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G19" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="H19" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>79</v>
+        <v>125</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>80</v>
+        <v>138</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>81</v>
+        <v>152</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>82</v>
+        <v>166</v>
       </c>
       <c r="M19" t="s">
-        <v>83</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="F20" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="G20" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="H20" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>80</v>
+        <v>139</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>82</v>
+        <v>167</v>
       </c>
       <c r="M20" t="s">
-        <v>83</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F21" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="G21" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="H21" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>81</v>
+        <v>154</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>82</v>
+        <v>168</v>
       </c>
       <c r="M21" t="s">
-        <v>83</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>